<commit_message>
fixed recurring credentials request in wrapper
</commit_message>
<xml_diff>
--- a/VM_Server_Script_Sequence.xlsx
+++ b/VM_Server_Script_Sequence.xlsx
@@ -1420,6 +1420,12 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -1435,12 +1441,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -1454,81 +1460,75 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1825,20 +1825,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="116" t="s">
+      <c r="A1" s="118" t="s">
         <v>156</v>
       </c>
-      <c r="B1" s="116"/>
-      <c r="C1" s="116"/>
-      <c r="D1" s="116"/>
-      <c r="E1" s="116"/>
-      <c r="F1" s="116"/>
+      <c r="B1" s="118"/>
+      <c r="C1" s="118"/>
+      <c r="D1" s="118"/>
+      <c r="E1" s="118"/>
+      <c r="F1" s="118"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="126" t="s">
+      <c r="A3" s="128" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="126"/>
+      <c r="B3" s="128"/>
       <c r="C3" s="1" t="s">
         <v>11</v>
       </c>
@@ -2335,24 +2335,24 @@
       <c r="F32" s="13"/>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A33" s="117" t="s">
+      <c r="A33" s="119" t="s">
         <v>57</v>
       </c>
-      <c r="B33" s="118"/>
-      <c r="C33" s="118"/>
-      <c r="D33" s="118"/>
-      <c r="E33" s="118"/>
-      <c r="F33" s="119"/>
+      <c r="B33" s="120"/>
+      <c r="C33" s="120"/>
+      <c r="D33" s="120"/>
+      <c r="E33" s="120"/>
+      <c r="F33" s="121"/>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34" s="4">
         <v>1</v>
       </c>
       <c r="B34" s="8"/>
-      <c r="C34" s="120"/>
-      <c r="D34" s="120"/>
-      <c r="E34" s="120"/>
-      <c r="F34" s="121"/>
+      <c r="C34" s="122"/>
+      <c r="D34" s="122"/>
+      <c r="E34" s="122"/>
+      <c r="F34" s="123"/>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35" s="4">
@@ -2361,12 +2361,12 @@
       <c r="B35" s="8" t="s">
         <v>45</v>
       </c>
-      <c r="C35" s="122" t="s">
+      <c r="C35" s="124" t="s">
         <v>175</v>
       </c>
-      <c r="D35" s="122"/>
-      <c r="E35" s="122"/>
-      <c r="F35" s="123"/>
+      <c r="D35" s="124"/>
+      <c r="E35" s="124"/>
+      <c r="F35" s="125"/>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36" s="4">
@@ -2375,38 +2375,38 @@
       <c r="B36" s="5" t="s">
         <v>166</v>
       </c>
-      <c r="C36" s="122"/>
-      <c r="D36" s="122"/>
-      <c r="E36" s="122"/>
-      <c r="F36" s="123"/>
+      <c r="C36" s="124"/>
+      <c r="D36" s="124"/>
+      <c r="E36" s="124"/>
+      <c r="F36" s="125"/>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37" s="4">
         <v>4</v>
       </c>
       <c r="B37" s="26"/>
-      <c r="C37" s="124"/>
-      <c r="D37" s="124"/>
-      <c r="E37" s="124"/>
-      <c r="F37" s="125"/>
+      <c r="C37" s="126"/>
+      <c r="D37" s="126"/>
+      <c r="E37" s="126"/>
+      <c r="F37" s="127"/>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="C38" s="115"/>
-      <c r="D38" s="115"/>
-      <c r="E38" s="115"/>
-      <c r="F38" s="115"/>
+      <c r="C38" s="117"/>
+      <c r="D38" s="117"/>
+      <c r="E38" s="117"/>
+      <c r="F38" s="117"/>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="C39" s="115"/>
-      <c r="D39" s="115"/>
-      <c r="E39" s="115"/>
-      <c r="F39" s="115"/>
+      <c r="C39" s="117"/>
+      <c r="D39" s="117"/>
+      <c r="E39" s="117"/>
+      <c r="F39" s="117"/>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="C40" s="115"/>
-      <c r="D40" s="115"/>
-      <c r="E40" s="115"/>
-      <c r="F40" s="115"/>
+      <c r="C40" s="117"/>
+      <c r="D40" s="117"/>
+      <c r="E40" s="117"/>
+      <c r="F40" s="117"/>
     </row>
   </sheetData>
   <mergeCells count="10">
@@ -2430,8 +2430,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:J52"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A38" zoomScale="106" zoomScaleNormal="106" workbookViewId="0">
-      <selection activeCell="C40" sqref="C40:I40"/>
+    <sheetView tabSelected="1" topLeftCell="A14" zoomScale="106" zoomScaleNormal="106" workbookViewId="0">
+      <selection activeCell="I23" sqref="I23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2868,7 +2868,7 @@
       <c r="H16" s="92" t="s">
         <v>151</v>
       </c>
-      <c r="I16" s="168" t="s">
+      <c r="I16" s="115" t="s">
         <v>240</v>
       </c>
       <c r="J16" s="91" t="s">
@@ -2894,7 +2894,7 @@
       <c r="H17" s="91" t="s">
         <v>151</v>
       </c>
-      <c r="I17" s="169"/>
+      <c r="I17" s="116"/>
       <c r="J17" s="91" t="s">
         <v>153</v>
       </c>
@@ -2924,7 +2924,7 @@
       <c r="H18" s="92" t="s">
         <v>151</v>
       </c>
-      <c r="I18" s="169" t="s">
+      <c r="I18" s="116" t="s">
         <v>232</v>
       </c>
       <c r="J18" s="91" t="s">
@@ -2956,7 +2956,7 @@
       <c r="H19" s="92" t="s">
         <v>151</v>
       </c>
-      <c r="I19" s="168" t="s">
+      <c r="I19" s="115" t="s">
         <v>240</v>
       </c>
       <c r="J19" s="91" t="s">
@@ -2988,7 +2988,7 @@
       <c r="H20" s="92" t="s">
         <v>151</v>
       </c>
-      <c r="I20" s="168" t="s">
+      <c r="I20" s="115" t="s">
         <v>240</v>
       </c>
       <c r="J20" s="91" t="s">
@@ -3018,7 +3018,7 @@
       <c r="H21" s="92" t="s">
         <v>151</v>
       </c>
-      <c r="I21" s="168" t="s">
+      <c r="I21" s="115" t="s">
         <v>240</v>
       </c>
       <c r="J21" s="91" t="s">
@@ -3262,192 +3262,192 @@
       </c>
     </row>
     <row r="33" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B33" s="130" t="s">
+      <c r="B33" s="132" t="s">
         <v>227</v>
       </c>
-      <c r="C33" s="131"/>
-      <c r="D33" s="131"/>
-      <c r="E33" s="131"/>
-      <c r="F33" s="131"/>
-      <c r="G33" s="131"/>
-      <c r="H33" s="131"/>
-      <c r="I33" s="131"/>
+      <c r="C33" s="133"/>
+      <c r="D33" s="133"/>
+      <c r="E33" s="133"/>
+      <c r="F33" s="133"/>
+      <c r="G33" s="133"/>
+      <c r="H33" s="133"/>
+      <c r="I33" s="133"/>
     </row>
     <row r="34" spans="2:9" ht="45.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B34" s="109" t="s">
         <v>84</v>
       </c>
-      <c r="C34" s="129" t="s">
+      <c r="C34" s="130" t="s">
         <v>229</v>
       </c>
-      <c r="D34" s="127"/>
-      <c r="E34" s="127"/>
-      <c r="F34" s="127"/>
-      <c r="G34" s="127"/>
-      <c r="H34" s="127"/>
-      <c r="I34" s="128"/>
+      <c r="D34" s="129"/>
+      <c r="E34" s="129"/>
+      <c r="F34" s="129"/>
+      <c r="G34" s="129"/>
+      <c r="H34" s="129"/>
+      <c r="I34" s="131"/>
     </row>
     <row r="35" spans="2:9" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B35" s="110" t="s">
         <v>85</v>
       </c>
-      <c r="C35" s="132" t="s">
+      <c r="C35" s="134" t="s">
         <v>228</v>
       </c>
-      <c r="D35" s="132"/>
-      <c r="E35" s="132"/>
-      <c r="F35" s="132"/>
-      <c r="G35" s="132"/>
-      <c r="H35" s="132"/>
-      <c r="I35" s="133"/>
+      <c r="D35" s="134"/>
+      <c r="E35" s="134"/>
+      <c r="F35" s="134"/>
+      <c r="G35" s="134"/>
+      <c r="H35" s="134"/>
+      <c r="I35" s="135"/>
     </row>
     <row r="36" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B36" s="103" t="s">
         <v>174</v>
       </c>
-      <c r="C36" s="134" t="s">
+      <c r="C36" s="136" t="s">
         <v>230</v>
       </c>
-      <c r="D36" s="122"/>
-      <c r="E36" s="122"/>
-      <c r="F36" s="122"/>
-      <c r="G36" s="122"/>
-      <c r="H36" s="122"/>
-      <c r="I36" s="123"/>
+      <c r="D36" s="124"/>
+      <c r="E36" s="124"/>
+      <c r="F36" s="124"/>
+      <c r="G36" s="124"/>
+      <c r="H36" s="124"/>
+      <c r="I36" s="125"/>
     </row>
     <row r="37" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B37" s="103" t="s">
         <v>172</v>
       </c>
-      <c r="C37" s="122" t="s">
+      <c r="C37" s="124" t="s">
         <v>231</v>
       </c>
-      <c r="D37" s="122"/>
-      <c r="E37" s="122"/>
-      <c r="F37" s="122"/>
-      <c r="G37" s="122"/>
-      <c r="H37" s="122"/>
-      <c r="I37" s="123"/>
+      <c r="D37" s="124"/>
+      <c r="E37" s="124"/>
+      <c r="F37" s="124"/>
+      <c r="G37" s="124"/>
+      <c r="H37" s="124"/>
+      <c r="I37" s="125"/>
     </row>
     <row r="38" spans="2:9" ht="150.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B38" s="103" t="s">
         <v>177</v>
       </c>
-      <c r="C38" s="127" t="s">
+      <c r="C38" s="129" t="s">
         <v>234</v>
       </c>
-      <c r="D38" s="122"/>
-      <c r="E38" s="122"/>
-      <c r="F38" s="122"/>
-      <c r="G38" s="122"/>
-      <c r="H38" s="122"/>
-      <c r="I38" s="123"/>
+      <c r="D38" s="124"/>
+      <c r="E38" s="124"/>
+      <c r="F38" s="124"/>
+      <c r="G38" s="124"/>
+      <c r="H38" s="124"/>
+      <c r="I38" s="125"/>
     </row>
     <row r="39" spans="2:9" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B39" s="103" t="s">
         <v>42</v>
       </c>
-      <c r="C39" s="127" t="s">
+      <c r="C39" s="129" t="s">
         <v>244</v>
       </c>
-      <c r="D39" s="127"/>
-      <c r="E39" s="127"/>
-      <c r="F39" s="127"/>
-      <c r="G39" s="127"/>
-      <c r="H39" s="127"/>
-      <c r="I39" s="128"/>
+      <c r="D39" s="129"/>
+      <c r="E39" s="129"/>
+      <c r="F39" s="129"/>
+      <c r="G39" s="129"/>
+      <c r="H39" s="129"/>
+      <c r="I39" s="131"/>
     </row>
     <row r="40" spans="2:9" ht="42.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B40" s="103" t="s">
         <v>36</v>
       </c>
-      <c r="C40" s="122" t="s">
+      <c r="C40" s="124" t="s">
         <v>237</v>
       </c>
-      <c r="D40" s="122"/>
-      <c r="E40" s="122"/>
-      <c r="F40" s="122"/>
-      <c r="G40" s="122"/>
-      <c r="H40" s="122"/>
-      <c r="I40" s="123"/>
+      <c r="D40" s="124"/>
+      <c r="E40" s="124"/>
+      <c r="F40" s="124"/>
+      <c r="G40" s="124"/>
+      <c r="H40" s="124"/>
+      <c r="I40" s="125"/>
     </row>
     <row r="41" spans="2:9" ht="90.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B41" s="103" t="s">
         <v>41</v>
       </c>
-      <c r="C41" s="127" t="s">
+      <c r="C41" s="129" t="s">
         <v>245</v>
       </c>
-      <c r="D41" s="122"/>
-      <c r="E41" s="122"/>
-      <c r="F41" s="122"/>
-      <c r="G41" s="122"/>
-      <c r="H41" s="122"/>
-      <c r="I41" s="123"/>
+      <c r="D41" s="124"/>
+      <c r="E41" s="124"/>
+      <c r="F41" s="124"/>
+      <c r="G41" s="124"/>
+      <c r="H41" s="124"/>
+      <c r="I41" s="125"/>
     </row>
     <row r="42" spans="2:9" ht="51" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B42" s="105" t="s">
         <v>83</v>
       </c>
-      <c r="C42" s="127" t="s">
+      <c r="C42" s="129" t="s">
         <v>243</v>
       </c>
-      <c r="D42" s="122"/>
-      <c r="E42" s="122"/>
-      <c r="F42" s="122"/>
-      <c r="G42" s="122"/>
-      <c r="H42" s="122"/>
-      <c r="I42" s="123"/>
+      <c r="D42" s="124"/>
+      <c r="E42" s="124"/>
+      <c r="F42" s="124"/>
+      <c r="G42" s="124"/>
+      <c r="H42" s="124"/>
+      <c r="I42" s="125"/>
     </row>
     <row r="43" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B43" s="3"/>
-      <c r="C43" s="122"/>
-      <c r="D43" s="122"/>
-      <c r="E43" s="122"/>
-      <c r="F43" s="122"/>
-      <c r="G43" s="122"/>
-      <c r="H43" s="122"/>
-      <c r="I43" s="123"/>
+      <c r="C43" s="124"/>
+      <c r="D43" s="124"/>
+      <c r="E43" s="124"/>
+      <c r="F43" s="124"/>
+      <c r="G43" s="124"/>
+      <c r="H43" s="124"/>
+      <c r="I43" s="125"/>
     </row>
     <row r="44" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B44" s="3"/>
-      <c r="C44" s="122"/>
-      <c r="D44" s="122"/>
-      <c r="E44" s="122"/>
-      <c r="F44" s="122"/>
-      <c r="G44" s="122"/>
-      <c r="H44" s="122"/>
-      <c r="I44" s="123"/>
+      <c r="C44" s="124"/>
+      <c r="D44" s="124"/>
+      <c r="E44" s="124"/>
+      <c r="F44" s="124"/>
+      <c r="G44" s="124"/>
+      <c r="H44" s="124"/>
+      <c r="I44" s="125"/>
     </row>
     <row r="45" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B45" s="3"/>
-      <c r="C45" s="122"/>
-      <c r="D45" s="122"/>
-      <c r="E45" s="122"/>
-      <c r="F45" s="122"/>
-      <c r="G45" s="122"/>
-      <c r="H45" s="122"/>
-      <c r="I45" s="123"/>
+      <c r="C45" s="124"/>
+      <c r="D45" s="124"/>
+      <c r="E45" s="124"/>
+      <c r="F45" s="124"/>
+      <c r="G45" s="124"/>
+      <c r="H45" s="124"/>
+      <c r="I45" s="125"/>
     </row>
     <row r="50" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B50" s="115"/>
-      <c r="C50" s="115"/>
-      <c r="D50" s="115"/>
-      <c r="E50" s="115"/>
-      <c r="F50" s="115"/>
-      <c r="G50" s="115"/>
-      <c r="H50" s="115"/>
-      <c r="I50" s="115"/>
+      <c r="B50" s="117"/>
+      <c r="C50" s="117"/>
+      <c r="D50" s="117"/>
+      <c r="E50" s="117"/>
+      <c r="F50" s="117"/>
+      <c r="G50" s="117"/>
+      <c r="H50" s="117"/>
+      <c r="I50" s="117"/>
     </row>
     <row r="51" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B51" s="95"/>
-      <c r="C51" s="115"/>
-      <c r="D51" s="115"/>
-      <c r="E51" s="115"/>
-      <c r="F51" s="115"/>
-      <c r="G51" s="115"/>
-      <c r="H51" s="115"/>
-      <c r="I51" s="115"/>
+      <c r="C51" s="117"/>
+      <c r="D51" s="117"/>
+      <c r="E51" s="117"/>
+      <c r="F51" s="117"/>
+      <c r="G51" s="117"/>
+      <c r="H51" s="117"/>
+      <c r="I51" s="117"/>
     </row>
     <row r="52" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B52" s="95"/>
@@ -3457,12 +3457,6 @@
     <sortCondition ref="B9:B28"/>
   </sortState>
   <mergeCells count="15">
-    <mergeCell ref="C38:I38"/>
-    <mergeCell ref="C34:I34"/>
-    <mergeCell ref="B33:I33"/>
-    <mergeCell ref="C35:I35"/>
-    <mergeCell ref="C36:I36"/>
-    <mergeCell ref="C37:I37"/>
     <mergeCell ref="C45:I45"/>
     <mergeCell ref="B50:I50"/>
     <mergeCell ref="C51:I51"/>
@@ -3472,6 +3466,12 @@
     <mergeCell ref="C42:I42"/>
     <mergeCell ref="C43:I43"/>
     <mergeCell ref="C44:I44"/>
+    <mergeCell ref="C38:I38"/>
+    <mergeCell ref="C34:I34"/>
+    <mergeCell ref="B33:I33"/>
+    <mergeCell ref="C35:I35"/>
+    <mergeCell ref="C36:I36"/>
+    <mergeCell ref="C37:I37"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -3513,11 +3513,11 @@
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" s="126" t="s">
+      <c r="A3" s="128" t="s">
         <v>60</v>
       </c>
-      <c r="B3" s="126"/>
-      <c r="C3" s="126"/>
+      <c r="B3" s="128"/>
+      <c r="C3" s="128"/>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
@@ -3741,15 +3741,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A1" s="149" t="s">
+      <c r="A1" s="152" t="s">
         <v>58</v>
       </c>
-      <c r="B1" s="149"/>
-      <c r="C1" s="149"/>
-      <c r="D1" s="149"/>
-      <c r="E1" s="149"/>
-      <c r="F1" s="149"/>
-      <c r="G1" s="149"/>
+      <c r="B1" s="152"/>
+      <c r="C1" s="152"/>
+      <c r="D1" s="152"/>
+      <c r="E1" s="152"/>
+      <c r="F1" s="152"/>
+      <c r="G1" s="152"/>
       <c r="H1" s="62" t="s">
         <v>92</v>
       </c>
@@ -3758,14 +3758,14 @@
       <c r="A2" s="29">
         <v>1</v>
       </c>
-      <c r="B2" s="157" t="s">
+      <c r="B2" s="138" t="s">
         <v>89</v>
       </c>
-      <c r="C2" s="158"/>
-      <c r="D2" s="158"/>
-      <c r="E2" s="158"/>
-      <c r="F2" s="158"/>
-      <c r="G2" s="158"/>
+      <c r="C2" s="139"/>
+      <c r="D2" s="139"/>
+      <c r="E2" s="139"/>
+      <c r="F2" s="139"/>
+      <c r="G2" s="139"/>
       <c r="H2" s="64" t="s">
         <v>87</v>
       </c>
@@ -3775,13 +3775,13 @@
         <v>2</v>
       </c>
       <c r="B3" s="31"/>
-      <c r="C3" s="156" t="s">
+      <c r="C3" s="137" t="s">
         <v>88</v>
       </c>
-      <c r="D3" s="120"/>
-      <c r="E3" s="120"/>
-      <c r="F3" s="120"/>
-      <c r="G3" s="120"/>
+      <c r="D3" s="122"/>
+      <c r="E3" s="122"/>
+      <c r="F3" s="122"/>
+      <c r="G3" s="122"/>
       <c r="H3" s="64" t="s">
         <v>91</v>
       </c>
@@ -3791,13 +3791,13 @@
         <v>3</v>
       </c>
       <c r="B4" s="33"/>
-      <c r="C4" s="163" t="s">
+      <c r="C4" s="140" t="s">
         <v>99</v>
       </c>
-      <c r="D4" s="164"/>
-      <c r="E4" s="164"/>
-      <c r="F4" s="164"/>
-      <c r="G4" s="164"/>
+      <c r="D4" s="141"/>
+      <c r="E4" s="141"/>
+      <c r="F4" s="141"/>
+      <c r="G4" s="141"/>
       <c r="H4" s="3" t="s">
         <v>99</v>
       </c>
@@ -3807,13 +3807,13 @@
         <v>4</v>
       </c>
       <c r="B5" s="33"/>
-      <c r="C5" s="147" t="s">
+      <c r="C5" s="142" t="s">
         <v>100</v>
       </c>
-      <c r="D5" s="148"/>
-      <c r="E5" s="148"/>
-      <c r="F5" s="148"/>
-      <c r="G5" s="148"/>
+      <c r="D5" s="143"/>
+      <c r="E5" s="143"/>
+      <c r="F5" s="143"/>
+      <c r="G5" s="143"/>
       <c r="H5" s="65" t="s">
         <v>170</v>
       </c>
@@ -3824,12 +3824,12 @@
       </c>
       <c r="B6" s="34"/>
       <c r="C6" s="27"/>
-      <c r="D6" s="165" t="s">
+      <c r="D6" s="144" t="s">
         <v>101</v>
       </c>
-      <c r="E6" s="166"/>
-      <c r="F6" s="166"/>
-      <c r="G6" s="166"/>
+      <c r="E6" s="145"/>
+      <c r="F6" s="145"/>
+      <c r="G6" s="145"/>
       <c r="H6" s="65" t="s">
         <v>170</v>
       </c>
@@ -3839,13 +3839,13 @@
         <v>6</v>
       </c>
       <c r="B7" s="36"/>
-      <c r="C7" s="167" t="s">
+      <c r="C7" s="146" t="s">
         <v>102</v>
       </c>
-      <c r="D7" s="167"/>
-      <c r="E7" s="167"/>
-      <c r="F7" s="167"/>
-      <c r="G7" s="157"/>
+      <c r="D7" s="146"/>
+      <c r="E7" s="146"/>
+      <c r="F7" s="146"/>
+      <c r="G7" s="138"/>
       <c r="H7" s="65" t="s">
         <v>170</v>
       </c>
@@ -3856,12 +3856,12 @@
       </c>
       <c r="B8" s="37"/>
       <c r="C8" s="38"/>
-      <c r="D8" s="156" t="s">
+      <c r="D8" s="137" t="s">
         <v>30</v>
       </c>
-      <c r="E8" s="120"/>
-      <c r="F8" s="120"/>
-      <c r="G8" s="120"/>
+      <c r="E8" s="122"/>
+      <c r="F8" s="122"/>
+      <c r="G8" s="122"/>
       <c r="H8" s="65" t="s">
         <v>170</v>
       </c>
@@ -3872,12 +3872,12 @@
       </c>
       <c r="B9" s="28"/>
       <c r="C9" s="39"/>
-      <c r="D9" s="156" t="s">
+      <c r="D9" s="137" t="s">
         <v>31</v>
       </c>
-      <c r="E9" s="120"/>
-      <c r="F9" s="120"/>
-      <c r="G9" s="120"/>
+      <c r="E9" s="122"/>
+      <c r="F9" s="122"/>
+      <c r="G9" s="122"/>
       <c r="H9" s="24" t="s">
         <v>31</v>
       </c>
@@ -3888,12 +3888,12 @@
       </c>
       <c r="B10" s="28"/>
       <c r="C10" s="39"/>
-      <c r="D10" s="156" t="s">
+      <c r="D10" s="137" t="s">
         <v>32</v>
       </c>
-      <c r="E10" s="120"/>
-      <c r="F10" s="120"/>
-      <c r="G10" s="120"/>
+      <c r="E10" s="122"/>
+      <c r="F10" s="122"/>
+      <c r="G10" s="122"/>
       <c r="H10" s="24" t="s">
         <v>32</v>
       </c>
@@ -3904,12 +3904,12 @@
       </c>
       <c r="B11" s="28"/>
       <c r="C11" s="39"/>
-      <c r="D11" s="156" t="s">
+      <c r="D11" s="137" t="s">
         <v>33</v>
       </c>
-      <c r="E11" s="120"/>
-      <c r="F11" s="120"/>
-      <c r="G11" s="120"/>
+      <c r="E11" s="122"/>
+      <c r="F11" s="122"/>
+      <c r="G11" s="122"/>
       <c r="H11" s="24" t="s">
         <v>33</v>
       </c>
@@ -3920,12 +3920,12 @@
       </c>
       <c r="B12" s="40"/>
       <c r="C12" s="41"/>
-      <c r="D12" s="157" t="s">
+      <c r="D12" s="138" t="s">
         <v>34</v>
       </c>
-      <c r="E12" s="158"/>
-      <c r="F12" s="158"/>
-      <c r="G12" s="158"/>
+      <c r="E12" s="139"/>
+      <c r="F12" s="139"/>
+      <c r="G12" s="139"/>
       <c r="H12" s="65" t="s">
         <v>171</v>
       </c>
@@ -3937,11 +3937,11 @@
       <c r="B13" s="42"/>
       <c r="C13" s="42"/>
       <c r="D13" s="17"/>
-      <c r="E13" s="156" t="s">
+      <c r="E13" s="137" t="s">
         <v>35</v>
       </c>
-      <c r="F13" s="120"/>
-      <c r="G13" s="120"/>
+      <c r="F13" s="122"/>
+      <c r="G13" s="122"/>
       <c r="H13" s="66" t="s">
         <v>172</v>
       </c>
@@ -3953,11 +3953,11 @@
       <c r="B14" s="43"/>
       <c r="C14" s="43"/>
       <c r="D14" s="18"/>
-      <c r="E14" s="156" t="s">
+      <c r="E14" s="137" t="s">
         <v>36</v>
       </c>
-      <c r="F14" s="120"/>
-      <c r="G14" s="120"/>
+      <c r="F14" s="122"/>
+      <c r="G14" s="122"/>
       <c r="H14" s="67" t="s">
         <v>36</v>
       </c>
@@ -3968,12 +3968,12 @@
       </c>
       <c r="B15" s="45"/>
       <c r="C15" s="46"/>
-      <c r="D15" s="157" t="s">
+      <c r="D15" s="138" t="s">
         <v>37</v>
       </c>
-      <c r="E15" s="158"/>
-      <c r="F15" s="158"/>
-      <c r="G15" s="158"/>
+      <c r="E15" s="139"/>
+      <c r="F15" s="139"/>
+      <c r="G15" s="139"/>
       <c r="H15" s="65" t="s">
         <v>170</v>
       </c>
@@ -3985,11 +3985,11 @@
       <c r="B16" s="47"/>
       <c r="C16" s="47"/>
       <c r="D16" s="20"/>
-      <c r="E16" s="156" t="s">
+      <c r="E16" s="137" t="s">
         <v>38</v>
       </c>
-      <c r="F16" s="120"/>
-      <c r="G16" s="120"/>
+      <c r="F16" s="122"/>
+      <c r="G16" s="122"/>
       <c r="H16" s="67" t="s">
         <v>38</v>
       </c>
@@ -4001,11 +4001,11 @@
       <c r="B17" s="48"/>
       <c r="C17" s="48"/>
       <c r="D17" s="21"/>
-      <c r="E17" s="156" t="s">
+      <c r="E17" s="137" t="s">
         <v>39</v>
       </c>
-      <c r="F17" s="120"/>
-      <c r="G17" s="120"/>
+      <c r="F17" s="122"/>
+      <c r="G17" s="122"/>
       <c r="H17" s="67" t="s">
         <v>39</v>
       </c>
@@ -4017,11 +4017,11 @@
       <c r="B18" s="49"/>
       <c r="C18" s="49"/>
       <c r="D18" s="22"/>
-      <c r="E18" s="156" t="s">
+      <c r="E18" s="137" t="s">
         <v>40</v>
       </c>
-      <c r="F18" s="120"/>
-      <c r="G18" s="120"/>
+      <c r="F18" s="122"/>
+      <c r="G18" s="122"/>
       <c r="H18" s="84" t="s">
         <v>173</v>
       </c>
@@ -4032,12 +4032,12 @@
       </c>
       <c r="B19" s="50"/>
       <c r="C19" s="51"/>
-      <c r="D19" s="157" t="s">
+      <c r="D19" s="138" t="s">
         <v>98</v>
       </c>
-      <c r="E19" s="158"/>
-      <c r="F19" s="158"/>
-      <c r="G19" s="158"/>
+      <c r="E19" s="139"/>
+      <c r="F19" s="139"/>
+      <c r="G19" s="139"/>
       <c r="H19" s="65" t="s">
         <v>137</v>
       </c>
@@ -4049,11 +4049,11 @@
       <c r="B20" s="50"/>
       <c r="C20" s="50"/>
       <c r="D20" s="19"/>
-      <c r="E20" s="157" t="s">
+      <c r="E20" s="138" t="s">
         <v>98</v>
       </c>
-      <c r="F20" s="158"/>
-      <c r="G20" s="158"/>
+      <c r="F20" s="139"/>
+      <c r="G20" s="139"/>
       <c r="H20" s="71" t="s">
         <v>136</v>
       </c>
@@ -4066,10 +4066,10 @@
       <c r="C21" s="48"/>
       <c r="D21" s="23"/>
       <c r="E21" s="20"/>
-      <c r="F21" s="156" t="s">
+      <c r="F21" s="137" t="s">
         <v>103</v>
       </c>
-      <c r="G21" s="120"/>
+      <c r="G21" s="122"/>
       <c r="H21" s="71" t="s">
         <v>136</v>
       </c>
@@ -4082,10 +4082,10 @@
       <c r="C22" s="48"/>
       <c r="D22" s="23"/>
       <c r="E22" s="21"/>
-      <c r="F22" s="156" t="s">
+      <c r="F22" s="137" t="s">
         <v>104</v>
       </c>
-      <c r="G22" s="120"/>
+      <c r="G22" s="122"/>
       <c r="H22" s="71" t="s">
         <v>136</v>
       </c>
@@ -4098,10 +4098,10 @@
       <c r="C23" s="48"/>
       <c r="D23" s="23"/>
       <c r="E23" s="21"/>
-      <c r="F23" s="156" t="s">
+      <c r="F23" s="137" t="s">
         <v>105</v>
       </c>
-      <c r="G23" s="120"/>
+      <c r="G23" s="122"/>
       <c r="H23" s="71" t="s">
         <v>136</v>
       </c>
@@ -4114,10 +4114,10 @@
       <c r="C24" s="48"/>
       <c r="D24" s="23"/>
       <c r="E24" s="21"/>
-      <c r="F24" s="156" t="s">
+      <c r="F24" s="137" t="s">
         <v>106</v>
       </c>
-      <c r="G24" s="120"/>
+      <c r="G24" s="122"/>
       <c r="H24" s="71" t="s">
         <v>136</v>
       </c>
@@ -4130,10 +4130,10 @@
       <c r="C25" s="48"/>
       <c r="D25" s="23"/>
       <c r="E25" s="21"/>
-      <c r="F25" s="156" t="s">
+      <c r="F25" s="137" t="s">
         <v>107</v>
       </c>
-      <c r="G25" s="120"/>
+      <c r="G25" s="122"/>
       <c r="H25" s="71" t="s">
         <v>136</v>
       </c>
@@ -4146,10 +4146,10 @@
       <c r="C26" s="48"/>
       <c r="D26" s="23"/>
       <c r="E26" s="21"/>
-      <c r="F26" s="156" t="s">
+      <c r="F26" s="137" t="s">
         <v>108</v>
       </c>
-      <c r="G26" s="120"/>
+      <c r="G26" s="122"/>
       <c r="H26" s="71" t="s">
         <v>136</v>
       </c>
@@ -4162,10 +4162,10 @@
       <c r="C27" s="48"/>
       <c r="D27" s="23"/>
       <c r="E27" s="21"/>
-      <c r="F27" s="156" t="s">
+      <c r="F27" s="137" t="s">
         <v>109</v>
       </c>
-      <c r="G27" s="120"/>
+      <c r="G27" s="122"/>
       <c r="H27" s="71" t="s">
         <v>136</v>
       </c>
@@ -4178,10 +4178,10 @@
       <c r="C28" s="48"/>
       <c r="D28" s="23"/>
       <c r="E28" s="21"/>
-      <c r="F28" s="156" t="s">
+      <c r="F28" s="137" t="s">
         <v>110</v>
       </c>
-      <c r="G28" s="120"/>
+      <c r="G28" s="122"/>
       <c r="H28" s="71" t="s">
         <v>136</v>
       </c>
@@ -4194,10 +4194,10 @@
       <c r="C29" s="48"/>
       <c r="D29" s="23"/>
       <c r="E29" s="21"/>
-      <c r="F29" s="156" t="s">
+      <c r="F29" s="137" t="s">
         <v>111</v>
       </c>
-      <c r="G29" s="120"/>
+      <c r="G29" s="122"/>
       <c r="H29" s="71" t="s">
         <v>136</v>
       </c>
@@ -4210,10 +4210,10 @@
       <c r="C30" s="48"/>
       <c r="D30" s="23"/>
       <c r="E30" s="21"/>
-      <c r="F30" s="156" t="s">
+      <c r="F30" s="137" t="s">
         <v>112</v>
       </c>
-      <c r="G30" s="120"/>
+      <c r="G30" s="122"/>
       <c r="H30" s="71" t="s">
         <v>136</v>
       </c>
@@ -4226,10 +4226,10 @@
       <c r="C31" s="48"/>
       <c r="D31" s="23"/>
       <c r="E31" s="21"/>
-      <c r="F31" s="156" t="s">
+      <c r="F31" s="137" t="s">
         <v>113</v>
       </c>
-      <c r="G31" s="120"/>
+      <c r="G31" s="122"/>
       <c r="H31" s="71" t="s">
         <v>136</v>
       </c>
@@ -4242,10 +4242,10 @@
       <c r="C32" s="48"/>
       <c r="D32" s="23"/>
       <c r="E32" s="21"/>
-      <c r="F32" s="156" t="s">
+      <c r="F32" s="137" t="s">
         <v>114</v>
       </c>
-      <c r="G32" s="120"/>
+      <c r="G32" s="122"/>
       <c r="H32" s="71" t="s">
         <v>136</v>
       </c>
@@ -4258,10 +4258,10 @@
       <c r="C33" s="48"/>
       <c r="D33" s="23"/>
       <c r="E33" s="21"/>
-      <c r="F33" s="156" t="s">
+      <c r="F33" s="137" t="s">
         <v>115</v>
       </c>
-      <c r="G33" s="120"/>
+      <c r="G33" s="122"/>
       <c r="H33" s="71" t="s">
         <v>136</v>
       </c>
@@ -4274,10 +4274,10 @@
       <c r="C34" s="48"/>
       <c r="D34" s="23"/>
       <c r="E34" s="21"/>
-      <c r="F34" s="156" t="s">
+      <c r="F34" s="137" t="s">
         <v>116</v>
       </c>
-      <c r="G34" s="120"/>
+      <c r="G34" s="122"/>
       <c r="H34" s="71" t="s">
         <v>136</v>
       </c>
@@ -4290,10 +4290,10 @@
       <c r="C35" s="48"/>
       <c r="D35" s="23"/>
       <c r="E35" s="21"/>
-      <c r="F35" s="156" t="s">
+      <c r="F35" s="137" t="s">
         <v>117</v>
       </c>
-      <c r="G35" s="120"/>
+      <c r="G35" s="122"/>
       <c r="H35" s="71" t="s">
         <v>136</v>
       </c>
@@ -4306,10 +4306,10 @@
       <c r="C36" s="48"/>
       <c r="D36" s="23"/>
       <c r="E36" s="21"/>
-      <c r="F36" s="156" t="s">
+      <c r="F36" s="137" t="s">
         <v>118</v>
       </c>
-      <c r="G36" s="120"/>
+      <c r="G36" s="122"/>
       <c r="H36" s="71" t="s">
         <v>136</v>
       </c>
@@ -4322,10 +4322,10 @@
       <c r="C37" s="48"/>
       <c r="D37" s="23"/>
       <c r="E37" s="21"/>
-      <c r="F37" s="156" t="s">
+      <c r="F37" s="137" t="s">
         <v>119</v>
       </c>
-      <c r="G37" s="120"/>
+      <c r="G37" s="122"/>
       <c r="H37" s="71" t="s">
         <v>136</v>
       </c>
@@ -4338,10 +4338,10 @@
       <c r="C38" s="48"/>
       <c r="D38" s="23"/>
       <c r="E38" s="21"/>
-      <c r="F38" s="156" t="s">
+      <c r="F38" s="137" t="s">
         <v>120</v>
       </c>
-      <c r="G38" s="120"/>
+      <c r="G38" s="122"/>
       <c r="H38" s="71" t="s">
         <v>136</v>
       </c>
@@ -4354,10 +4354,10 @@
       <c r="C39" s="48"/>
       <c r="D39" s="52"/>
       <c r="E39" s="22"/>
-      <c r="F39" s="156" t="s">
+      <c r="F39" s="137" t="s">
         <v>121</v>
       </c>
-      <c r="G39" s="120"/>
+      <c r="G39" s="122"/>
       <c r="H39" s="71" t="s">
         <v>136</v>
       </c>
@@ -4368,12 +4368,12 @@
       </c>
       <c r="B40" s="47"/>
       <c r="C40" s="53"/>
-      <c r="D40" s="156" t="s">
+      <c r="D40" s="137" t="s">
         <v>41</v>
       </c>
-      <c r="E40" s="120"/>
-      <c r="F40" s="120"/>
-      <c r="G40" s="120"/>
+      <c r="E40" s="122"/>
+      <c r="F40" s="122"/>
+      <c r="G40" s="122"/>
       <c r="H40" s="24" t="s">
         <v>41</v>
       </c>
@@ -4384,12 +4384,12 @@
       </c>
       <c r="B41" s="48"/>
       <c r="C41" s="54"/>
-      <c r="D41" s="156" t="s">
+      <c r="D41" s="137" t="s">
         <v>42</v>
       </c>
-      <c r="E41" s="120"/>
-      <c r="F41" s="120"/>
-      <c r="G41" s="120"/>
+      <c r="E41" s="122"/>
+      <c r="F41" s="122"/>
+      <c r="G41" s="122"/>
       <c r="H41" s="24" t="s">
         <v>42</v>
       </c>
@@ -4400,12 +4400,12 @@
       </c>
       <c r="B42" s="49"/>
       <c r="C42" s="55"/>
-      <c r="D42" s="157" t="s">
+      <c r="D42" s="138" t="s">
         <v>43</v>
       </c>
-      <c r="E42" s="158"/>
-      <c r="F42" s="158"/>
-      <c r="G42" s="158"/>
+      <c r="E42" s="139"/>
+      <c r="F42" s="139"/>
+      <c r="G42" s="139"/>
       <c r="H42" s="64" t="s">
         <v>83</v>
       </c>
@@ -4417,11 +4417,11 @@
       <c r="B43" s="47"/>
       <c r="C43" s="47"/>
       <c r="D43" s="20"/>
-      <c r="E43" s="156" t="s">
+      <c r="E43" s="137" t="s">
         <v>93</v>
       </c>
-      <c r="F43" s="120"/>
-      <c r="G43" s="120"/>
+      <c r="F43" s="122"/>
+      <c r="G43" s="122"/>
       <c r="H43" s="64" t="s">
         <v>83</v>
       </c>
@@ -4433,11 +4433,11 @@
       <c r="B44" s="49"/>
       <c r="C44" s="49"/>
       <c r="D44" s="22"/>
-      <c r="E44" s="157" t="s">
+      <c r="E44" s="138" t="s">
         <v>94</v>
       </c>
-      <c r="F44" s="158"/>
-      <c r="G44" s="158"/>
+      <c r="F44" s="139"/>
+      <c r="G44" s="139"/>
       <c r="H44" s="64" t="s">
         <v>83</v>
       </c>
@@ -4450,10 +4450,10 @@
       <c r="C45" s="48"/>
       <c r="D45" s="23"/>
       <c r="E45" s="56"/>
-      <c r="F45" s="160" t="s">
+      <c r="F45" s="149" t="s">
         <v>93</v>
       </c>
-      <c r="G45" s="156"/>
+      <c r="G45" s="137"/>
       <c r="H45" s="64" t="s">
         <v>83</v>
       </c>
@@ -4466,10 +4466,10 @@
       <c r="C46" s="48"/>
       <c r="D46" s="23"/>
       <c r="E46" s="21"/>
-      <c r="F46" s="161" t="s">
+      <c r="F46" s="150" t="s">
         <v>122</v>
       </c>
-      <c r="G46" s="162"/>
+      <c r="G46" s="151"/>
       <c r="H46" s="64" t="s">
         <v>83</v>
       </c>
@@ -4530,10 +4530,10 @@
       <c r="C50" s="48"/>
       <c r="D50" s="23"/>
       <c r="E50" s="21"/>
-      <c r="F50" s="161" t="s">
+      <c r="F50" s="150" t="s">
         <v>126</v>
       </c>
-      <c r="G50" s="162"/>
+      <c r="G50" s="151"/>
       <c r="H50" s="64" t="s">
         <v>83</v>
       </c>
@@ -4578,10 +4578,10 @@
       <c r="C53" s="48"/>
       <c r="D53" s="23"/>
       <c r="E53" s="21"/>
-      <c r="F53" s="161" t="s">
+      <c r="F53" s="150" t="s">
         <v>128</v>
       </c>
-      <c r="G53" s="162"/>
+      <c r="G53" s="151"/>
       <c r="H53" s="64" t="s">
         <v>83</v>
       </c>
@@ -4626,10 +4626,10 @@
       <c r="C56" s="48"/>
       <c r="D56" s="23"/>
       <c r="E56" s="21"/>
-      <c r="F56" s="161" t="s">
+      <c r="F56" s="150" t="s">
         <v>130</v>
       </c>
-      <c r="G56" s="162"/>
+      <c r="G56" s="151"/>
       <c r="H56" s="64" t="s">
         <v>83</v>
       </c>
@@ -4674,10 +4674,10 @@
       <c r="C59" s="48"/>
       <c r="D59" s="23"/>
       <c r="E59" s="21"/>
-      <c r="F59" s="150" t="s">
+      <c r="F59" s="153" t="s">
         <v>132</v>
       </c>
-      <c r="G59" s="151"/>
+      <c r="G59" s="154"/>
       <c r="H59" s="64" t="s">
         <v>83</v>
       </c>
@@ -4722,10 +4722,10 @@
       <c r="C62" s="48"/>
       <c r="D62" s="23"/>
       <c r="E62" s="21"/>
-      <c r="F62" s="150" t="s">
+      <c r="F62" s="153" t="s">
         <v>134</v>
       </c>
-      <c r="G62" s="151"/>
+      <c r="G62" s="154"/>
       <c r="H62" s="64" t="s">
         <v>83</v>
       </c>
@@ -4769,11 +4769,11 @@
       <c r="B65" s="50"/>
       <c r="C65" s="50"/>
       <c r="D65" s="19"/>
-      <c r="E65" s="152" t="s">
+      <c r="E65" s="155" t="s">
         <v>95</v>
       </c>
-      <c r="F65" s="152"/>
-      <c r="G65" s="153"/>
+      <c r="F65" s="155"/>
+      <c r="G65" s="147"/>
       <c r="H65" s="64" t="s">
         <v>83</v>
       </c>
@@ -4784,12 +4784,12 @@
       </c>
       <c r="B66" s="50"/>
       <c r="C66" s="51"/>
-      <c r="D66" s="154" t="s">
+      <c r="D66" s="156" t="s">
         <v>44</v>
       </c>
-      <c r="E66" s="155"/>
-      <c r="F66" s="155"/>
-      <c r="G66" s="155"/>
+      <c r="E66" s="157"/>
+      <c r="F66" s="157"/>
+      <c r="G66" s="157"/>
       <c r="H66" s="65" t="s">
         <v>137</v>
       </c>
@@ -4802,10 +4802,10 @@
       <c r="C67" s="50"/>
       <c r="D67" s="60"/>
       <c r="E67" s="61"/>
-      <c r="F67" s="153" t="s">
+      <c r="F67" s="147" t="s">
         <v>59</v>
       </c>
-      <c r="G67" s="159"/>
+      <c r="G67" s="148"/>
       <c r="H67" s="65" t="s">
         <v>137</v>
       </c>
@@ -4816,12 +4816,12 @@
       </c>
       <c r="B68" s="50"/>
       <c r="C68" s="51"/>
-      <c r="D68" s="153" t="s">
+      <c r="D68" s="147" t="s">
         <v>52</v>
       </c>
-      <c r="E68" s="159"/>
-      <c r="F68" s="159"/>
-      <c r="G68" s="159"/>
+      <c r="E68" s="148"/>
+      <c r="F68" s="148"/>
+      <c r="G68" s="148"/>
       <c r="H68" s="66" t="s">
         <v>174</v>
       </c>
@@ -4847,180 +4847,161 @@
       </c>
     </row>
     <row r="75" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A75" s="126" t="s">
+      <c r="A75" s="128" t="s">
         <v>57</v>
       </c>
-      <c r="B75" s="126"/>
-      <c r="C75" s="126"/>
-      <c r="D75" s="126"/>
-      <c r="E75" s="126"/>
-      <c r="F75" s="126"/>
-      <c r="G75" s="126"/>
-      <c r="H75" s="126"/>
+      <c r="B75" s="128"/>
+      <c r="C75" s="128"/>
+      <c r="D75" s="128"/>
+      <c r="E75" s="128"/>
+      <c r="F75" s="128"/>
+      <c r="G75" s="128"/>
+      <c r="H75" s="128"/>
     </row>
     <row r="76" spans="1:8" s="63" customFormat="1" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A76" s="135" t="s">
+      <c r="A76" s="166" t="s">
         <v>100</v>
       </c>
-      <c r="B76" s="136"/>
-      <c r="C76" s="136"/>
-      <c r="D76" s="136"/>
-      <c r="E76" s="127" t="s">
+      <c r="B76" s="167"/>
+      <c r="C76" s="167"/>
+      <c r="D76" s="167"/>
+      <c r="E76" s="129" t="s">
         <v>138</v>
       </c>
-      <c r="F76" s="127"/>
-      <c r="G76" s="127"/>
-      <c r="H76" s="128"/>
+      <c r="F76" s="129"/>
+      <c r="G76" s="129"/>
+      <c r="H76" s="131"/>
     </row>
     <row r="77" spans="1:8" s="63" customFormat="1" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A77" s="135" t="s">
+      <c r="A77" s="166" t="s">
         <v>101</v>
       </c>
-      <c r="B77" s="136"/>
-      <c r="C77" s="136"/>
-      <c r="D77" s="136"/>
-      <c r="E77" s="127" t="s">
+      <c r="B77" s="167"/>
+      <c r="C77" s="167"/>
+      <c r="D77" s="167"/>
+      <c r="E77" s="129" t="s">
         <v>139</v>
       </c>
-      <c r="F77" s="127"/>
-      <c r="G77" s="127"/>
-      <c r="H77" s="128"/>
+      <c r="F77" s="129"/>
+      <c r="G77" s="129"/>
+      <c r="H77" s="131"/>
     </row>
     <row r="78" spans="1:8" s="63" customFormat="1" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A78" s="135" t="s">
+      <c r="A78" s="166" t="s">
         <v>102</v>
       </c>
-      <c r="B78" s="136"/>
-      <c r="C78" s="136"/>
-      <c r="D78" s="136"/>
-      <c r="E78" s="127" t="s">
+      <c r="B78" s="167"/>
+      <c r="C78" s="167"/>
+      <c r="D78" s="167"/>
+      <c r="E78" s="129" t="s">
         <v>140</v>
       </c>
-      <c r="F78" s="127"/>
-      <c r="G78" s="127"/>
-      <c r="H78" s="128"/>
+      <c r="F78" s="129"/>
+      <c r="G78" s="129"/>
+      <c r="H78" s="131"/>
     </row>
     <row r="79" spans="1:8" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A79" s="137" t="s">
+      <c r="A79" s="168" t="s">
         <v>30</v>
       </c>
-      <c r="B79" s="138"/>
-      <c r="C79" s="138"/>
-      <c r="D79" s="138"/>
-      <c r="E79" s="122" t="s">
+      <c r="B79" s="169"/>
+      <c r="C79" s="169"/>
+      <c r="D79" s="169"/>
+      <c r="E79" s="124" t="s">
         <v>141</v>
       </c>
-      <c r="F79" s="122"/>
-      <c r="G79" s="122"/>
-      <c r="H79" s="123"/>
+      <c r="F79" s="124"/>
+      <c r="G79" s="124"/>
+      <c r="H79" s="125"/>
     </row>
     <row r="80" spans="1:8" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A80" s="141" t="s">
+      <c r="A80" s="158" t="s">
         <v>34</v>
       </c>
-      <c r="B80" s="142"/>
-      <c r="C80" s="142"/>
-      <c r="D80" s="142"/>
-      <c r="E80" s="139" t="s">
+      <c r="B80" s="159"/>
+      <c r="C80" s="159"/>
+      <c r="D80" s="159"/>
+      <c r="E80" s="164" t="s">
         <v>96</v>
       </c>
-      <c r="F80" s="139"/>
-      <c r="G80" s="139"/>
-      <c r="H80" s="140"/>
+      <c r="F80" s="164"/>
+      <c r="G80" s="164"/>
+      <c r="H80" s="165"/>
     </row>
     <row r="81" spans="1:8" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A81" s="143" t="s">
+      <c r="A81" s="160" t="s">
         <v>37</v>
       </c>
-      <c r="B81" s="144"/>
-      <c r="C81" s="144"/>
-      <c r="D81" s="144"/>
-      <c r="E81" s="127" t="s">
+      <c r="B81" s="161"/>
+      <c r="C81" s="161"/>
+      <c r="D81" s="161"/>
+      <c r="E81" s="129" t="s">
         <v>96</v>
       </c>
-      <c r="F81" s="127"/>
-      <c r="G81" s="127"/>
-      <c r="H81" s="128"/>
+      <c r="F81" s="129"/>
+      <c r="G81" s="129"/>
+      <c r="H81" s="131"/>
     </row>
     <row r="82" spans="1:8" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A82" s="145" t="s">
+      <c r="A82" s="162" t="s">
         <v>44</v>
       </c>
-      <c r="B82" s="146"/>
-      <c r="C82" s="146"/>
-      <c r="D82" s="146"/>
-      <c r="E82" s="127" t="s">
+      <c r="B82" s="163"/>
+      <c r="C82" s="163"/>
+      <c r="D82" s="163"/>
+      <c r="E82" s="129" t="s">
         <v>97</v>
       </c>
-      <c r="F82" s="127"/>
-      <c r="G82" s="127"/>
-      <c r="H82" s="128"/>
+      <c r="F82" s="129"/>
+      <c r="G82" s="129"/>
+      <c r="H82" s="131"/>
     </row>
     <row r="83" spans="1:8" ht="49.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A83" s="147" t="s">
+      <c r="A83" s="142" t="s">
         <v>98</v>
       </c>
-      <c r="B83" s="148"/>
-      <c r="C83" s="148"/>
-      <c r="D83" s="148"/>
-      <c r="E83" s="127" t="s">
+      <c r="B83" s="143"/>
+      <c r="C83" s="143"/>
+      <c r="D83" s="143"/>
+      <c r="E83" s="129" t="s">
         <v>142</v>
       </c>
-      <c r="F83" s="127"/>
-      <c r="G83" s="127"/>
-      <c r="H83" s="128"/>
+      <c r="F83" s="129"/>
+      <c r="G83" s="129"/>
+      <c r="H83" s="131"/>
     </row>
     <row r="84" spans="1:8" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A84" s="134"/>
-      <c r="B84" s="122"/>
-      <c r="C84" s="122"/>
-      <c r="D84" s="122"/>
-      <c r="E84" s="122"/>
-      <c r="F84" s="122"/>
-      <c r="G84" s="122"/>
-      <c r="H84" s="123"/>
+      <c r="A84" s="136"/>
+      <c r="B84" s="124"/>
+      <c r="C84" s="124"/>
+      <c r="D84" s="124"/>
+      <c r="E84" s="124"/>
+      <c r="F84" s="124"/>
+      <c r="G84" s="124"/>
+      <c r="H84" s="125"/>
     </row>
   </sheetData>
   <mergeCells count="75">
-    <mergeCell ref="E13:G13"/>
-    <mergeCell ref="B2:G2"/>
-    <mergeCell ref="C3:G3"/>
-    <mergeCell ref="C4:G4"/>
-    <mergeCell ref="C5:G5"/>
-    <mergeCell ref="D6:G6"/>
-    <mergeCell ref="C7:G7"/>
-    <mergeCell ref="D8:G8"/>
-    <mergeCell ref="D9:G9"/>
-    <mergeCell ref="D10:G10"/>
-    <mergeCell ref="D11:G11"/>
-    <mergeCell ref="D12:G12"/>
-    <mergeCell ref="F25:G25"/>
-    <mergeCell ref="E14:G14"/>
-    <mergeCell ref="D15:G15"/>
-    <mergeCell ref="E16:G16"/>
-    <mergeCell ref="E17:G17"/>
-    <mergeCell ref="E18:G18"/>
-    <mergeCell ref="D19:G19"/>
-    <mergeCell ref="E20:G20"/>
-    <mergeCell ref="F21:G21"/>
-    <mergeCell ref="F22:G22"/>
-    <mergeCell ref="F23:G23"/>
-    <mergeCell ref="F24:G24"/>
-    <mergeCell ref="F37:G37"/>
-    <mergeCell ref="F26:G26"/>
-    <mergeCell ref="F27:G27"/>
-    <mergeCell ref="F28:G28"/>
-    <mergeCell ref="F29:G29"/>
-    <mergeCell ref="F30:G30"/>
-    <mergeCell ref="F31:G31"/>
-    <mergeCell ref="F67:G67"/>
-    <mergeCell ref="D68:G68"/>
-    <mergeCell ref="E44:G44"/>
-    <mergeCell ref="F45:G45"/>
-    <mergeCell ref="F46:G46"/>
-    <mergeCell ref="F50:G50"/>
-    <mergeCell ref="F53:G53"/>
-    <mergeCell ref="F56:G56"/>
+    <mergeCell ref="E84:H84"/>
+    <mergeCell ref="A76:D76"/>
+    <mergeCell ref="A77:D77"/>
+    <mergeCell ref="A78:D78"/>
+    <mergeCell ref="A79:D79"/>
+    <mergeCell ref="E76:H76"/>
+    <mergeCell ref="E77:H77"/>
+    <mergeCell ref="E78:H78"/>
+    <mergeCell ref="E79:H79"/>
+    <mergeCell ref="A84:D84"/>
+    <mergeCell ref="E75:H75"/>
+    <mergeCell ref="E80:H80"/>
+    <mergeCell ref="E81:H81"/>
+    <mergeCell ref="E82:H82"/>
+    <mergeCell ref="E83:H83"/>
+    <mergeCell ref="A75:D75"/>
+    <mergeCell ref="A80:D80"/>
+    <mergeCell ref="A81:D81"/>
+    <mergeCell ref="A82:D82"/>
+    <mergeCell ref="A83:D83"/>
     <mergeCell ref="A1:G1"/>
     <mergeCell ref="F59:G59"/>
     <mergeCell ref="F62:G62"/>
@@ -5037,26 +5018,45 @@
     <mergeCell ref="F34:G34"/>
     <mergeCell ref="F35:G35"/>
     <mergeCell ref="F36:G36"/>
-    <mergeCell ref="A75:D75"/>
-    <mergeCell ref="A80:D80"/>
-    <mergeCell ref="A81:D81"/>
-    <mergeCell ref="A82:D82"/>
-    <mergeCell ref="A83:D83"/>
-    <mergeCell ref="E75:H75"/>
-    <mergeCell ref="E80:H80"/>
-    <mergeCell ref="E81:H81"/>
-    <mergeCell ref="E82:H82"/>
-    <mergeCell ref="E83:H83"/>
-    <mergeCell ref="E84:H84"/>
-    <mergeCell ref="A76:D76"/>
-    <mergeCell ref="A77:D77"/>
-    <mergeCell ref="A78:D78"/>
-    <mergeCell ref="A79:D79"/>
-    <mergeCell ref="E76:H76"/>
-    <mergeCell ref="E77:H77"/>
-    <mergeCell ref="E78:H78"/>
-    <mergeCell ref="E79:H79"/>
-    <mergeCell ref="A84:D84"/>
+    <mergeCell ref="F67:G67"/>
+    <mergeCell ref="D68:G68"/>
+    <mergeCell ref="E44:G44"/>
+    <mergeCell ref="F45:G45"/>
+    <mergeCell ref="F46:G46"/>
+    <mergeCell ref="F50:G50"/>
+    <mergeCell ref="F53:G53"/>
+    <mergeCell ref="F56:G56"/>
+    <mergeCell ref="F37:G37"/>
+    <mergeCell ref="F26:G26"/>
+    <mergeCell ref="F27:G27"/>
+    <mergeCell ref="F28:G28"/>
+    <mergeCell ref="F29:G29"/>
+    <mergeCell ref="F30:G30"/>
+    <mergeCell ref="F31:G31"/>
+    <mergeCell ref="F25:G25"/>
+    <mergeCell ref="E14:G14"/>
+    <mergeCell ref="D15:G15"/>
+    <mergeCell ref="E16:G16"/>
+    <mergeCell ref="E17:G17"/>
+    <mergeCell ref="E18:G18"/>
+    <mergeCell ref="D19:G19"/>
+    <mergeCell ref="E20:G20"/>
+    <mergeCell ref="F21:G21"/>
+    <mergeCell ref="F22:G22"/>
+    <mergeCell ref="F23:G23"/>
+    <mergeCell ref="F24:G24"/>
+    <mergeCell ref="E13:G13"/>
+    <mergeCell ref="B2:G2"/>
+    <mergeCell ref="C3:G3"/>
+    <mergeCell ref="C4:G4"/>
+    <mergeCell ref="C5:G5"/>
+    <mergeCell ref="D6:G6"/>
+    <mergeCell ref="C7:G7"/>
+    <mergeCell ref="D8:G8"/>
+    <mergeCell ref="D9:G9"/>
+    <mergeCell ref="D10:G10"/>
+    <mergeCell ref="D11:G11"/>
+    <mergeCell ref="D12:G12"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>